<commit_message>
Start to delete GlobaleVars
</commit_message>
<xml_diff>
--- a/Gestion projet.xlsx
+++ b/Gestion projet.xlsx
@@ -337,17 +337,17 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -647,10 +647,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Liste_de_tâches" displayName="Liste_de_tâches" ref="B4:G9" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="B4:G9"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Tâche" dataDxfId="2"/>
-    <tableColumn id="3" name="Priorité " dataDxfId="3"/>
-    <tableColumn id="4" name="État " dataDxfId="5"/>
-    <tableColumn id="6" name="Date Proposition" dataDxfId="4"/>
+    <tableColumn id="1" name="Tâche" dataDxfId="5"/>
+    <tableColumn id="3" name="Priorité " dataDxfId="4"/>
+    <tableColumn id="4" name="État " dataDxfId="3"/>
+    <tableColumn id="6" name="Date Proposition" dataDxfId="2"/>
     <tableColumn id="5" name="% achevé" dataDxfId="1"/>
     <tableColumn id="10" name="Notes" dataDxfId="0"/>
   </tableColumns>
@@ -907,7 +907,7 @@
   <dimension ref="B1:G10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -960,7 +960,7 @@
         <v>42781</v>
       </c>
       <c r="F5" s="3">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>19</v>
@@ -1016,7 +1016,7 @@
         <v>42781</v>
       </c>
       <c r="F8" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="14"/>
     </row>
@@ -1101,6 +1101,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>